<commit_message>
how is each map different from the others
</commit_message>
<xml_diff>
--- a/maps to make.xlsx
+++ b/maps to make.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>map</t>
   </si>
@@ -84,28 +84,32 @@
     <t>india</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">demographic and health survey
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>with prevR</t>
-    </r>
+    <t>chooses colors based on statistically significant differences</t>
+  </si>
+  <si>
+    <t>different from others because #1</t>
+  </si>
+  <si>
+    <t>different from others because #2</t>
+  </si>
+  <si>
+    <t>demographic and health survey</t>
+  </si>
+  <si>
+    <t>uses the prevR package</t>
+  </si>
+  <si>
+    <t>computes small area population weights from census microdata rather than from a prepared file</t>
+  </si>
+  <si>
+    <t>??? Do we also convert this to ggplot2?  Or is that too hard?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,14 +121,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -467,47 +463,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="2" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -515,31 +520,39 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -547,31 +560,39 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -580,19 +601,21 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>20</v>
@@ -603,8 +626,14 @@
       <c r="G7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -613,12 +642,14 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
-    <hyperlink ref="G3" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>

</xml_diff>